<commit_message>
Save progress before rebase
</commit_message>
<xml_diff>
--- a/PatientReport.xlsx
+++ b/PatientReport.xlsx
@@ -38,6 +38,108 @@
     <t>Dr. Alice Smith (Physiotherapy)</t>
   </si>
   <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Patient 11</t>
+  </si>
+  <si>
+    <t>Address 11</t>
+  </si>
+  <si>
+    <t>555-0011</t>
+  </si>
+  <si>
+    <t>2025-05-01 10:00:07</t>
+  </si>
+  <si>
+    <t>Booked</t>
+  </si>
+  <si>
+    <t>Dr. Alice Smith (Rehabilitation)</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Patient 8</t>
+  </si>
+  <si>
+    <t>Address 8</t>
+  </si>
+  <si>
+    <t>555-008</t>
+  </si>
+  <si>
+    <t>2025-05-01 13:00:07</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Patient 5</t>
+  </si>
+  <si>
+    <t>Address 5</t>
+  </si>
+  <si>
+    <t>555-005</t>
+  </si>
+  <si>
+    <t>2025-05-01 16:00:07</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Patient 10</t>
+  </si>
+  <si>
+    <t>Address 10</t>
+  </si>
+  <si>
+    <t>555-0010</t>
+  </si>
+  <si>
+    <t>2025-05-01 19:00:07</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Patient 3</t>
+  </si>
+  <si>
+    <t>Address 3</t>
+  </si>
+  <si>
+    <t>555-003</t>
+  </si>
+  <si>
+    <t>2025-05-01 22:00:07</t>
+  </si>
+  <si>
+    <t>2025-05-08 10:00:07</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Patient 13</t>
+  </si>
+  <si>
+    <t>Address 13</t>
+  </si>
+  <si>
+    <t>555-0013</t>
+  </si>
+  <si>
+    <t>2025-05-08 13:00:07</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
     <t>7</t>
   </si>
   <si>
@@ -50,82 +152,55 @@
     <t>555-007</t>
   </si>
   <si>
-    <t>2025-05-01 10:00:38</t>
-  </si>
-  <si>
-    <t>Booked</t>
-  </si>
-  <si>
-    <t>Dr. Alice Smith (Rehabilitation)</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>Patient 11</t>
-  </si>
-  <si>
-    <t>Address 11</t>
-  </si>
-  <si>
-    <t>555-0011</t>
-  </si>
-  <si>
-    <t>2025-05-01 13:00:38</t>
+    <t>2025-05-08 16:00:07</t>
+  </si>
+  <si>
+    <t>2025-05-08 19:00:07</t>
   </si>
   <si>
     <t>Attended</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Patient 5</t>
-  </si>
-  <si>
-    <t>Address 5</t>
-  </si>
-  <si>
-    <t>555-005</t>
-  </si>
-  <si>
-    <t>2025-05-01 16:00:38</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>Patient 10</t>
-  </si>
-  <si>
-    <t>Address 10</t>
-  </si>
-  <si>
-    <t>555-0010</t>
-  </si>
-  <si>
-    <t>2025-05-01 19:00:38</t>
-  </si>
-  <si>
-    <t>2025-05-01 22:00:38</t>
-  </si>
-  <si>
-    <t>Cancelled</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>Patient 13</t>
-  </si>
-  <si>
-    <t>Address 13</t>
-  </si>
-  <si>
-    <t>555-0013</t>
-  </si>
-  <si>
-    <t>2025-05-08 10:00:38</t>
+    <t>2025-05-08 22:00:07</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Patient 4</t>
+  </si>
+  <si>
+    <t>Address 4</t>
+  </si>
+  <si>
+    <t>555-004</t>
+  </si>
+  <si>
+    <t>2025-05-15 10:00:07</t>
+  </si>
+  <si>
+    <t>2025-05-15 13:00:07</t>
+  </si>
+  <si>
+    <t>2025-05-15 16:00:07</t>
+  </si>
+  <si>
+    <t>2025-05-15 19:00:07</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Patient 12</t>
+  </si>
+  <si>
+    <t>Address 12</t>
+  </si>
+  <si>
+    <t>555-0012</t>
+  </si>
+  <si>
+    <t>2025-05-15 22:00:07</t>
   </si>
   <si>
     <t>15</t>
@@ -140,10 +215,67 @@
     <t>555-0015</t>
   </si>
   <si>
-    <t>2025-05-08 13:00:38</t>
-  </si>
-  <si>
-    <t>2025-05-08 16:00:38</t>
+    <t>2025-05-22 10:00:07</t>
+  </si>
+  <si>
+    <t>2025-05-22 13:00:07</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Patient 2</t>
+  </si>
+  <si>
+    <t>Address 2</t>
+  </si>
+  <si>
+    <t>555-002</t>
+  </si>
+  <si>
+    <t>2025-05-22 16:00:07</t>
+  </si>
+  <si>
+    <t>2025-05-22 19:00:07</t>
+  </si>
+  <si>
+    <t>2025-05-22 22:00:07</t>
+  </si>
+  <si>
+    <t>Dr. Bob Jones (Osteopathy)</t>
+  </si>
+  <si>
+    <t>Dr. Bob Jones (Physiotherapy)</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Patient 1</t>
+  </si>
+  <si>
+    <t>Address 1</t>
+  </si>
+  <si>
+    <t>555-001</t>
+  </si>
+  <si>
+    <t>Dr. Carol White (Rehabilitation)</t>
+  </si>
+  <si>
+    <t>Dr. Carol White (Sports Therapy)</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Patient 6</t>
+  </si>
+  <si>
+    <t>Address 6</t>
+  </si>
+  <si>
+    <t>555-006</t>
   </si>
   <si>
     <t>14</t>
@@ -158,75 +290,6 @@
     <t>555-0014</t>
   </si>
   <si>
-    <t>2025-05-08 19:00:38</t>
-  </si>
-  <si>
-    <t>2025-05-08 22:00:38</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>Patient 6</t>
-  </si>
-  <si>
-    <t>Address 6</t>
-  </si>
-  <si>
-    <t>555-006</t>
-  </si>
-  <si>
-    <t>2025-05-15 10:00:38</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Patient 4</t>
-  </si>
-  <si>
-    <t>Address 4</t>
-  </si>
-  <si>
-    <t>555-004</t>
-  </si>
-  <si>
-    <t>2025-05-15 13:00:38</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>Patient 8</t>
-  </si>
-  <si>
-    <t>Address 8</t>
-  </si>
-  <si>
-    <t>555-008</t>
-  </si>
-  <si>
-    <t>2025-05-15 16:00:38</t>
-  </si>
-  <si>
-    <t>2025-05-15 19:00:38</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Patient 3</t>
-  </si>
-  <si>
-    <t>Address 3</t>
-  </si>
-  <si>
-    <t>555-003</t>
-  </si>
-  <si>
-    <t>2025-05-15 22:00:38</t>
-  </si>
-  <si>
     <t>9</t>
   </si>
   <si>
@@ -237,69 +300,6 @@
   </si>
   <si>
     <t>555-009</t>
-  </si>
-  <si>
-    <t>2025-05-22 10:00:38</t>
-  </si>
-  <si>
-    <t>2025-05-22 13:00:38</t>
-  </si>
-  <si>
-    <t>2025-05-22 16:00:38</t>
-  </si>
-  <si>
-    <t>2025-05-22 19:00:38</t>
-  </si>
-  <si>
-    <t>2025-05-22 22:00:38</t>
-  </si>
-  <si>
-    <t>Dr. Bob Jones (Osteopathy)</t>
-  </si>
-  <si>
-    <t>Dr. Bob Jones (Physiotherapy)</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Patient 2</t>
-  </si>
-  <si>
-    <t>Address 2</t>
-  </si>
-  <si>
-    <t>555-002</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Patient 1</t>
-  </si>
-  <si>
-    <t>Address 1</t>
-  </si>
-  <si>
-    <t>555-001</t>
-  </si>
-  <si>
-    <t>Dr. Carol White (Rehabilitation)</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>Patient 12</t>
-  </si>
-  <si>
-    <t>Address 12</t>
-  </si>
-  <si>
-    <t>555-0012</t>
-  </si>
-  <si>
-    <t>Dr. Carol White (Sports Therapy)</t>
   </si>
   <si>
     <t>Dr. Alice Smith (Massage)</t>
@@ -446,7 +446,7 @@
         <v>19</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4">
@@ -454,19 +454,19 @@
         <v>7</v>
       </c>
       <c r="B4" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="D4" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="E4" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="F4" t="s" s="0">
         <v>24</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>25</v>
       </c>
       <c r="G4" t="s" s="0">
         <v>13</v>
@@ -477,19 +477,19 @@
         <v>14</v>
       </c>
       <c r="B5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="D5" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="E5" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="F5" t="s" s="0">
         <v>29</v>
-      </c>
-      <c r="F5" t="s" s="0">
-        <v>30</v>
       </c>
       <c r="G5" t="s" s="0">
         <v>13</v>
@@ -500,22 +500,22 @@
         <v>7</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7">
@@ -523,22 +523,22 @@
         <v>7</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="E7" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="F7" t="s" s="0">
-        <v>37</v>
-      </c>
       <c r="G7" t="s" s="0">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
@@ -546,22 +546,22 @@
         <v>14</v>
       </c>
       <c r="B8" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="C8" t="s" s="0">
+      <c r="E8" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="D8" t="s" s="0">
+      <c r="F8" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="E8" t="s" s="0">
+      <c r="G8" t="s" s="0">
         <v>41</v>
-      </c>
-      <c r="F8" t="s" s="0">
-        <v>42</v>
-      </c>
-      <c r="G8" t="s" s="0">
-        <v>13</v>
       </c>
     </row>
     <row r="9">
@@ -569,22 +569,22 @@
         <v>7</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F9" t="s" s="0">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G9" t="s" s="0">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10">
@@ -592,22 +592,22 @@
         <v>14</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F10" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="F10" t="s" s="0">
+      <c r="G10" t="s" s="0">
         <v>48</v>
-      </c>
-      <c r="G10" t="s" s="0">
-        <v>32</v>
       </c>
     </row>
     <row r="11">
@@ -615,22 +615,22 @@
         <v>7</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F11" t="s" s="0">
         <v>49</v>
       </c>
       <c r="G11" t="s" s="0">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12">
@@ -653,7 +653,7 @@
         <v>54</v>
       </c>
       <c r="G12" t="s" s="0">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13">
@@ -661,22 +661,22 @@
         <v>14</v>
       </c>
       <c r="B13" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="F13" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="C13" t="s" s="0">
-        <v>56</v>
-      </c>
-      <c r="D13" t="s" s="0">
-        <v>57</v>
-      </c>
-      <c r="E13" t="s" s="0">
-        <v>58</v>
-      </c>
-      <c r="F13" t="s" s="0">
-        <v>59</v>
-      </c>
       <c r="G13" t="s" s="0">
-        <v>13</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14">
@@ -684,22 +684,22 @@
         <v>7</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="E14" t="s" s="0">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="F14" t="s" s="0">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="G14" t="s" s="0">
-        <v>20</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15">
@@ -707,19 +707,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="C15" t="s" s="0">
+      <c r="D15" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="D15" t="s" s="0">
+      <c r="E15" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="E15" t="s" s="0">
-        <v>24</v>
-      </c>
       <c r="F15" t="s" s="0">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="G15" t="s" s="0">
         <v>13</v>
@@ -730,22 +730,22 @@
         <v>7</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D16" t="s" s="0">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E16" t="s" s="0">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="F16" t="s" s="0">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="G16" t="s" s="0">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17">
@@ -753,22 +753,22 @@
         <v>7</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D17" t="s" s="0">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="E17" t="s" s="0">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="F17" t="s" s="0">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="G17" t="s" s="0">
-        <v>20</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18">
@@ -776,22 +776,22 @@
         <v>14</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="E18" t="s" s="0">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="F18" t="s" s="0">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="G18" t="s" s="0">
-        <v>13</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19">
@@ -799,19 +799,19 @@
         <v>7</v>
       </c>
       <c r="B19" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="C19" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="D19" t="s" s="0">
         <v>71</v>
       </c>
-      <c r="C19" t="s" s="0">
+      <c r="E19" t="s" s="0">
         <v>72</v>
       </c>
-      <c r="D19" t="s" s="0">
+      <c r="F19" t="s" s="0">
         <v>73</v>
-      </c>
-      <c r="E19" t="s" s="0">
-        <v>74</v>
-      </c>
-      <c r="F19" t="s" s="0">
-        <v>77</v>
       </c>
       <c r="G19" t="s" s="0">
         <v>13</v>
@@ -822,19 +822,19 @@
         <v>14</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D20" t="s" s="0">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E20" t="s" s="0">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="F20" t="s" s="0">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G20" t="s" s="0">
         <v>13</v>
@@ -845,341 +845,341 @@
         <v>7</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s" s="0">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D21" t="s" s="0">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E21" t="s" s="0">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="F21" t="s" s="0">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G21" t="s" s="0">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D22" t="s" s="0">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E22" t="s" s="0">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F22" t="s" s="0">
         <v>12</v>
       </c>
       <c r="G22" t="s" s="0">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D23" t="s" s="0">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E23" t="s" s="0">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="F23" t="s" s="0">
         <v>19</v>
       </c>
       <c r="G23" t="s" s="0">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="D24" t="s" s="0">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="E24" t="s" s="0">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="F24" t="s" s="0">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G24" t="s" s="0">
-        <v>13</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="C25" t="s" s="0">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="D25" t="s" s="0">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="E25" t="s" s="0">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="F25" t="s" s="0">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G25" t="s" s="0">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="C26" t="s" s="0">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="D26" t="s" s="0">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="E26" t="s" s="0">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="F26" t="s" s="0">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G26" t="s" s="0">
-        <v>13</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="C27" t="s" s="0">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="D27" t="s" s="0">
-        <v>88</v>
+        <v>22</v>
       </c>
       <c r="E27" t="s" s="0">
-        <v>89</v>
+        <v>23</v>
       </c>
       <c r="F27" t="s" s="0">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G27" t="s" s="0">
-        <v>32</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="C28" t="s" s="0">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="D28" t="s" s="0">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="E28" t="s" s="0">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="F28" t="s" s="0">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G28" t="s" s="0">
-        <v>13</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C29" t="s" s="0">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D29" t="s" s="0">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="E29" t="s" s="0">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="F29" t="s" s="0">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G29" t="s" s="0">
-        <v>20</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C30" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="D30" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="E30" t="s" s="0">
         <v>81</v>
       </c>
-      <c r="B30" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="C30" t="s" s="0">
-        <v>72</v>
-      </c>
-      <c r="D30" t="s" s="0">
-        <v>73</v>
-      </c>
-      <c r="E30" t="s" s="0">
-        <v>74</v>
-      </c>
       <c r="F30" t="s" s="0">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G30" t="s" s="0">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>71</v>
+        <v>15</v>
       </c>
       <c r="C31" t="s" s="0">
-        <v>72</v>
+        <v>16</v>
       </c>
       <c r="D31" t="s" s="0">
-        <v>73</v>
+        <v>17</v>
       </c>
       <c r="E31" t="s" s="0">
-        <v>74</v>
+        <v>18</v>
       </c>
       <c r="F31" t="s" s="0">
         <v>49</v>
       </c>
       <c r="G31" t="s" s="0">
-        <v>13</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="C32" t="s" s="0">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="D32" t="s" s="0">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="E32" t="s" s="0">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="F32" t="s" s="0">
         <v>54</v>
       </c>
       <c r="G32" t="s" s="0">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="C33" t="s" s="0">
-        <v>72</v>
+        <v>9</v>
       </c>
       <c r="D33" t="s" s="0">
-        <v>73</v>
+        <v>10</v>
       </c>
       <c r="E33" t="s" s="0">
-        <v>74</v>
+        <v>11</v>
       </c>
       <c r="F33" t="s" s="0">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G33" t="s" s="0">
-        <v>20</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C34" t="s" s="0">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D34" t="s" s="0">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E34" t="s" s="0">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F34" t="s" s="0">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="G34" t="s" s="0">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="B35" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C35" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="D35" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="E35" t="s" s="0">
         <v>81</v>
       </c>
-      <c r="B35" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="C35" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="D35" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="E35" t="s" s="0">
-        <v>29</v>
-      </c>
       <c r="F35" t="s" s="0">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="G35" t="s" s="0">
         <v>13</v>
@@ -1187,45 +1187,45 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C36" t="s" s="0">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="D36" t="s" s="0">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="E36" t="s" s="0">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="F36" t="s" s="0">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="G36" t="s" s="0">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="C37" t="s" s="0">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="D37" t="s" s="0">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="E37" t="s" s="0">
-        <v>89</v>
+        <v>53</v>
       </c>
       <c r="F37" t="s" s="0">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="G37" t="s" s="0">
         <v>13</v>
@@ -1233,22 +1233,22 @@
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C38" t="s" s="0">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D38" t="s" s="0">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E38" t="s" s="0">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="F38" t="s" s="0">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="G38" t="s" s="0">
         <v>13</v>
@@ -1256,68 +1256,68 @@
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="C39" t="s" s="0">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D39" t="s" s="0">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="E39" t="s" s="0">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="F39" t="s" s="0">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G39" t="s" s="0">
-        <v>13</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="C40" t="s" s="0">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="D40" t="s" s="0">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="E40" t="s" s="0">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="F40" t="s" s="0">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G40" t="s" s="0">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="B41" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C41" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="D41" t="s" s="0">
         <v>80</v>
       </c>
-      <c r="B41" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="C41" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="D41" t="s" s="0">
-        <v>35</v>
-      </c>
       <c r="E41" t="s" s="0">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="F41" t="s" s="0">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G41" t="s" s="0">
         <v>13</v>
@@ -1325,42 +1325,42 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="C42" t="s" s="0">
-        <v>92</v>
+        <v>59</v>
       </c>
       <c r="D42" t="s" s="0">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="E42" t="s" s="0">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="F42" t="s" s="0">
         <v>12</v>
       </c>
       <c r="G42" t="s" s="0">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="C43" t="s" s="0">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="D43" t="s" s="0">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="E43" t="s" s="0">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="F43" t="s" s="0">
         <v>19</v>
@@ -1371,22 +1371,22 @@
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C44" t="s" s="0">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D44" t="s" s="0">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E44" t="s" s="0">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F44" t="s" s="0">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G44" t="s" s="0">
         <v>13</v>
@@ -1394,91 +1394,91 @@
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B45" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="C45" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="D45" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="C45" t="s" s="0">
+      <c r="E45" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="D45" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="E45" t="s" s="0">
-        <v>41</v>
-      </c>
       <c r="F45" t="s" s="0">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G45" t="s" s="0">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="C46" t="s" s="0">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="D46" t="s" s="0">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="E46" t="s" s="0">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="F46" t="s" s="0">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G46" t="s" s="0">
-        <v>13</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="C47" t="s" s="0">
+        <v>89</v>
+      </c>
+      <c r="D47" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="B47" t="s" s="0">
-        <v>44</v>
-      </c>
-      <c r="C47" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="D47" t="s" s="0">
-        <v>46</v>
-      </c>
       <c r="E47" t="s" s="0">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="F47" t="s" s="0">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G47" t="s" s="0">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="C48" t="s" s="0">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="D48" t="s" s="0">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="E48" t="s" s="0">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="F48" t="s" s="0">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G48" t="s" s="0">
         <v>13</v>
@@ -1486,137 +1486,137 @@
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="C49" t="s" s="0">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="D49" t="s" s="0">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="E49" t="s" s="0">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="F49" t="s" s="0">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G49" t="s" s="0">
-        <v>13</v>
+        <v>41</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="C50" t="s" s="0">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="D50" t="s" s="0">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="E50" t="s" s="0">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="F50" t="s" s="0">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G50" t="s" s="0">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="C51" t="s" s="0">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="D51" t="s" s="0">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="E51" t="s" s="0">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="F51" t="s" s="0">
         <v>49</v>
       </c>
       <c r="G51" t="s" s="0">
-        <v>20</v>
+        <v>41</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="C52" t="s" s="0">
-        <v>87</v>
+        <v>31</v>
       </c>
       <c r="D52" t="s" s="0">
-        <v>88</v>
+        <v>32</v>
       </c>
       <c r="E52" t="s" s="0">
-        <v>89</v>
+        <v>33</v>
       </c>
       <c r="F52" t="s" s="0">
         <v>54</v>
       </c>
       <c r="G52" t="s" s="0">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B53" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C53" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D53" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E53" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F53" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="C53" t="s" s="0">
-        <v>56</v>
-      </c>
-      <c r="D53" t="s" s="0">
-        <v>57</v>
-      </c>
-      <c r="E53" t="s" s="0">
-        <v>58</v>
-      </c>
-      <c r="F53" t="s" s="0">
-        <v>59</v>
-      </c>
       <c r="G53" t="s" s="0">
-        <v>20</v>
+        <v>41</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C54" t="s" s="0">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D54" t="s" s="0">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E54" t="s" s="0">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="F54" t="s" s="0">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="G54" t="s" s="0">
         <v>13</v>
@@ -1624,22 +1624,22 @@
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="C55" t="s" s="0">
-        <v>92</v>
+        <v>59</v>
       </c>
       <c r="D55" t="s" s="0">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="E55" t="s" s="0">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="F55" t="s" s="0">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="G55" t="s" s="0">
         <v>13</v>
@@ -1647,140 +1647,140 @@
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C56" t="s" s="0">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="D56" t="s" s="0">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E56" t="s" s="0">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="F56" t="s" s="0">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="G56" t="s" s="0">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="C57" t="s" s="0">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="D57" t="s" s="0">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="E57" t="s" s="0">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="F57" t="s" s="0">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="G57" t="s" s="0">
-        <v>13</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>91</v>
+        <v>42</v>
       </c>
       <c r="C58" t="s" s="0">
-        <v>92</v>
+        <v>43</v>
       </c>
       <c r="D58" t="s" s="0">
-        <v>93</v>
+        <v>44</v>
       </c>
       <c r="E58" t="s" s="0">
-        <v>94</v>
+        <v>45</v>
       </c>
       <c r="F58" t="s" s="0">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="G58" t="s" s="0">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C59" t="s" s="0">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D59" t="s" s="0">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E59" t="s" s="0">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="F59" t="s" s="0">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G59" t="s" s="0">
-        <v>13</v>
+        <v>48</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="C60" t="s" s="0">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="D60" t="s" s="0">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="E60" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="F60" t="s" s="0">
         <v>74</v>
       </c>
-      <c r="F60" t="s" s="0">
-        <v>78</v>
-      </c>
       <c r="G60" t="s" s="0">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="C61" t="s" s="0">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="D61" t="s" s="0">
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="E61" t="s" s="0">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="F61" t="s" s="0">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G61" t="s" s="0">
-        <v>13</v>
+        <v>48</v>
       </c>
     </row>
     <row r="62">
@@ -1788,22 +1788,22 @@
         <v>96</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C62" t="s" s="0">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D62" t="s" s="0">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E62" t="s" s="0">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F62" t="s" s="0">
         <v>12</v>
       </c>
       <c r="G62" t="s" s="0">
-        <v>20</v>
+        <v>48</v>
       </c>
     </row>
     <row r="65">
@@ -1819,7 +1819,7 @@
         <v>99</v>
       </c>
       <c r="B66" t="n" s="0">
-        <v>16.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="67">
@@ -1835,7 +1835,7 @@
         <v>101</v>
       </c>
       <c r="B68" t="n" s="0">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>